<commit_message>
refactor: modify temperature coeffs table
</commit_message>
<xml_diff>
--- a/data/processed/MS7001EA/T.xlsx
+++ b/data/processed/MS7001EA/T.xlsx
@@ -3,7 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="TA-E" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="TA" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="TB" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="TC" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="TD" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="TE" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,24 +15,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Tamb</t>
   </si>
   <si>
-    <t>Output %</t>
+    <t>Output</t>
   </si>
   <si>
-    <t>HR %</t>
+    <t>HR</t>
   </si>
   <si>
-    <t>HC %</t>
+    <t>HC</t>
   </si>
   <si>
     <t xml:space="preserve">Tx </t>
   </si>
   <si>
-    <t>ExFlow %</t>
+    <t>ExFlow</t>
   </si>
 </sst>
 </file>
@@ -114,9 +118,6 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -130,6 +131,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -139,6 +143,22 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -353,18 +373,6 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
@@ -373,248 +381,540 @@
       <c r="B2" s="4">
         <v>1.1439</v>
       </c>
-      <c r="C2" s="4">
-        <v>0.99455</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1.13767</v>
-      </c>
-      <c r="E2" s="5">
-        <v>-36.3</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1.11306</v>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>8.0</v>
       </c>
       <c r="B3" s="4">
         <v>1.14095</v>
       </c>
-      <c r="C3" s="4">
-        <v>0.98302</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1.12158</v>
-      </c>
-      <c r="E3" s="5">
-        <v>-36.39</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1.10654</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>19.0</v>
       </c>
       <c r="B4" s="4">
         <v>1.11022</v>
       </c>
-      <c r="C4" s="4">
-        <v>0.9852</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.09379</v>
-      </c>
-      <c r="E4" s="5">
-        <v>-27.95</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.08157</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>20.0</v>
       </c>
       <c r="B5" s="4">
         <v>1.12458</v>
       </c>
-      <c r="C5" s="4">
-        <v>0.97996</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.10204</v>
-      </c>
-      <c r="E5" s="5">
-        <v>-31.49</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.09171</v>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>40.0</v>
       </c>
       <c r="B6" s="4">
         <v>1.06261</v>
       </c>
-      <c r="C6" s="4">
-        <v>0.98783</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1.04968</v>
-      </c>
-      <c r="E6" s="5">
-        <v>-15.4</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1.04455</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>59.0</v>
       </c>
       <c r="B7" s="4">
         <v>1.0</v>
       </c>
-      <c r="C7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1.0</v>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>70.0</v>
       </c>
       <c r="B8" s="4">
         <v>0.96156</v>
       </c>
-      <c r="C8" s="4">
-        <v>1.00917</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.97038</v>
-      </c>
-      <c r="E8" s="5">
-        <v>8.14</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.97391</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>80.0</v>
       </c>
       <c r="B9" s="4">
         <v>0.92623</v>
       </c>
-      <c r="C9" s="4">
-        <v>1.0189</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.94374</v>
-      </c>
-      <c r="E9" s="5">
-        <v>15.65</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.94987</v>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>95.0</v>
       </c>
       <c r="B10" s="4">
         <v>0.87251</v>
       </c>
-      <c r="C10" s="4">
-        <v>1.0367</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.90407</v>
-      </c>
-      <c r="E10" s="5">
-        <v>27.78</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.91196</v>
-      </c>
     </row>
     <row r="11">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>110.0</v>
       </c>
       <c r="B11" s="4">
         <v>0.81927</v>
       </c>
-      <c r="C11" s="4">
+    </row>
+    <row r="15">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="6"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="6"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="6"/>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="6"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="6"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="6"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="6"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="6"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="6"/>
+      <c r="C27" s="9"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>-10.0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.99455</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.98302</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.9852</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.97996</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5">
+        <v>40.0</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.98783</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5">
+        <v>59.0</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>70.0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.00917</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1.0189</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5">
+        <v>95.0</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1.0367</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5">
+        <v>110.0</v>
+      </c>
+      <c r="B11" s="4">
         <v>1.05725</v>
       </c>
-      <c r="D11" s="4">
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>-10.0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.13767</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.12158</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.09379</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.10204</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5">
+        <v>40.0</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1.04968</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5">
+        <v>59.0</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>70.0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.97038</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.94374</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5">
+        <v>95.0</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.90407</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5">
+        <v>110.0</v>
+      </c>
+      <c r="B11" s="4">
         <v>0.86618</v>
       </c>
-      <c r="E11" s="5">
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>-10.0</v>
+      </c>
+      <c r="B2" s="10">
+        <v>-36.3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="B3" s="10">
+        <v>-36.39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="B4" s="10">
+        <v>-27.95</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="B5" s="10">
+        <v>-31.49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5">
+        <v>40.0</v>
+      </c>
+      <c r="B6" s="10">
+        <v>-15.4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5">
+        <v>59.0</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>70.0</v>
+      </c>
+      <c r="B8" s="10">
+        <v>8.14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="B9" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5">
+        <v>95.0</v>
+      </c>
+      <c r="B10" s="10">
+        <v>27.78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5">
+        <v>110.0</v>
+      </c>
+      <c r="B11" s="10">
         <v>40.69</v>
       </c>
-      <c r="F11" s="4">
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>-10.0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.11306</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.10654</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.08157</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.09171</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5">
+        <v>40.0</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1.04455</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5">
+        <v>59.0</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>70.0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.97391</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.94987</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5">
+        <v>95.0</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.91196</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5">
+        <v>110.0</v>
+      </c>
+      <c r="B11" s="4">
         <v>0.87321</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="7"/>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="7"/>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="7"/>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="7"/>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22">
-      <c r="B22" s="7"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23">
-      <c r="B23" s="7"/>
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24">
-      <c r="B24" s="7"/>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26">
-      <c r="B26" s="7"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27">
-      <c r="B27" s="7"/>
-      <c r="C27" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>